<commit_message>
final version without folders formatting
</commit_message>
<xml_diff>
--- a/backend/downloads/excel_values.xlsx
+++ b/backend/downloads/excel_values.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8,235,50</t>
+          <t>8235,50</t>
         </is>
       </c>
     </row>
@@ -572,7 +572,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4,944,27</t>
+          <t>4944,27</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>602201</t>
+          <t>601100</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2,242,03</t>
+          <t>2242,03</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>602202</t>
+          <t>602201</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -638,22 +638,49 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>602202</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>878318</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Achat MB 878318</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>34,89</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13/07/2024</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>602612</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>878318</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Achat MB 878318</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>34,89</t>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>878318</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Achat MB 878318</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>95,24</t>
         </is>
       </c>
     </row>

</xml_diff>